<commit_message>
Finished the SetUpController and setup form
</commit_message>
<xml_diff>
--- a/Documents/Client.xlsx
+++ b/Documents/Client.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="24">
   <si>
     <t>First Name</t>
   </si>
@@ -213,9 +213,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
@@ -555,7 +556,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9865D423-BCD0-47D6-86B0-3945943A592B}">
-  <dimension ref="A1:E27"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
@@ -927,6 +928,23 @@
         <v>23</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="s" s="13">
+        <v>14</v>
+      </c>
+      <c r="B28" t="s" s="13">
+        <v>14</v>
+      </c>
+      <c r="C28" t="s" s="13">
+        <v>14</v>
+      </c>
+      <c r="D28" t="s" s="13">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s" s="13">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>